<commit_message>
Clean example folder and module
</commit_message>
<xml_diff>
--- a/Example_Systems/Input_data_explained/Energy_share_requirement.xlsx
+++ b/Example_Systems/Input_data_explained/Energy_share_requirement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/abdelrahman_ayad_mail_mcgill_ca/Documents/McGill-PhD-Work/MITEI/GenX/Example_Systems/Input_data_explained/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/D/GenX/Code/misc/annoted_excel/Fwd__GenX_Excel_Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6B8418C0-B8A7-5149-AB57-7ED767E0A469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CC7C1D5-2104-3942-92CD-4FAA88CFE55B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8418C0-B8A7-5149-AB57-7ED767E0A469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32940" yWindow="500" windowWidth="34600" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy_share_requirement" sheetId="1" r:id="rId1"/>
@@ -573,17 +573,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -943,33 +943,30 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="C1:D1048576"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>